<commit_message>
Started improving GPS code. Verified IMU and baro work together
</commit_message>
<xml_diff>
--- a/module_pin_record.xlsx
+++ b/module_pin_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5DF922-E8DE-43D6-BAE1-9F79FD177BBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5E782-F974-46A3-A75A-18C34034EC6A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1185" windowWidth="10350" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Module/Pins</t>
   </si>
@@ -442,10 +442,10 @@
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +572,12 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
       <c r="R3" t="s">
         <v>31</v>
       </c>
@@ -582,6 +588,18 @@
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed GPS/demon code. Made SD writer function
</commit_message>
<xml_diff>
--- a/module_pin_record.xlsx
+++ b/module_pin_record.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5E782-F974-46A3-A75A-18C34034EC6A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A9398C-F1EC-4BF2-ACC6-AA67907F9543}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Module/Pins</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>y?</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +623,7 @@
         <v>31</v>
       </c>
       <c r="AA7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -630,7 +633,7 @@
       <c r="T8" t="s">
         <v>31</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="X8" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added better logging. Added camera and RTC.
</commit_message>
<xml_diff>
--- a/module_pin_record.xlsx
+++ b/module_pin_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A9398C-F1EC-4BF2-ACC6-AA67907F9543}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D993D304-51E6-4076-9EA5-FD3D88B24D8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Module/Pins</t>
   </si>
   <si>
-    <t>Barometer</t>
-  </si>
-  <si>
     <t>RST</t>
   </si>
   <si>
@@ -125,6 +122,15 @@
   </si>
   <si>
     <t>y?</t>
+  </si>
+  <si>
+    <t>Barometer BMP280</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>SCK-&gt;SCL</t>
   </si>
 </sst>
 </file>
@@ -442,18 +448,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomRight" activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -474,63 +480,63 @@
     <col min="30" max="30" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
       </c>
       <c r="T1">
         <v>4</v>
@@ -557,94 +563,100 @@
         <v>13</v>
       </c>
       <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA7" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="Y7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="T8" t="s">
+        <v>30</v>
+      </c>
+      <c r="X8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="T8" t="s">
-        <v>31</v>
-      </c>
-      <c r="X8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in audio, and rgb led
</commit_message>
<xml_diff>
--- a/module_pin_record.xlsx
+++ b/module_pin_record.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D993D304-51E6-4076-9EA5-FD3D88B24D8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CFFAC7-3D8C-4D36-84AB-4F290A5987BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Module/Pins</t>
   </si>
@@ -115,9 +116,6 @@
     <t>RTC</t>
   </si>
   <si>
-    <t>Audio</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -131,6 +129,27 @@
   </si>
   <si>
     <t>SCK-&gt;SCL</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>Audio buzzer</t>
+  </si>
+  <si>
+    <t>size of photo [kb]</t>
+  </si>
+  <si>
+    <t>size of SD card [Gb]</t>
+  </si>
+  <si>
+    <t>Length of time between photos [millis]</t>
+  </si>
+  <si>
+    <t>Total # photos that can be taken</t>
+  </si>
+  <si>
+    <t>Total length of flight that can be recorded [min]</t>
   </si>
 </sst>
 </file>
@@ -448,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF4" sqref="AF4"/>
+      <selection pane="bottomRight" activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +591,7 @@
         <v>21</v>
       </c>
       <c r="AF1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -582,22 +601,22 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AF3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -605,16 +624,16 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -632,10 +651,10 @@
         <v>26</v>
       </c>
       <c r="Y7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -643,10 +662,10 @@
         <v>27</v>
       </c>
       <c r="T8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -656,7 +675,78 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="W10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCDA486-89BA-4218-9F9D-8E64E4F0799C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <f>B2*(1000000000)/(B1*1000)</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <f>(B4*B3/1000)/60</f>
+        <v>666.66666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Final flight code -Added raw data from flight
</commit_message>
<xml_diff>
--- a/module_pin_record.xlsx
+++ b/module_pin_record.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA69A86-B505-4ED6-9F61-5A6460D0C871}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEDFEDD-31CC-46ED-B1B7-07952B00699A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Module/Pins</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>y?</t>
   </si>
   <si>
     <t>Barometer BMP280</t>
@@ -485,7 +482,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +600,7 @@
         <v>21</v>
       </c>
       <c r="AF1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -611,12 +608,12 @@
         <v>22</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -632,7 +629,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="AF3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -673,9 +670,6 @@
       <c r="Y7" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -697,7 +691,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W10" s="1"/>
       <c r="Z10" t="s">
@@ -706,7 +700,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V11" t="s">
         <v>29</v>
@@ -736,7 +730,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1">
         <v>50</v>
@@ -744,7 +738,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -752,7 +746,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -760,7 +754,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <f>B2*(1000000000)/(B1*1000)</f>
@@ -769,7 +763,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <f>(B4*B3/1000)/60</f>

</xml_diff>